<commit_message>
Regenerated Event Summary outputs
Added 6 practitioner examples
CIFMM-2585
</commit_message>
<xml_diff>
--- a/output/EventSummary/organization-dh-base-1.xlsx
+++ b/output/EventSummary/organization-dh-base-1.xlsx
@@ -153,7 +153,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}org-1:The organization SHALL at least have a name or an identifier, and possibly more than one {(identifier.count() + name.count()) &gt; 0}</t>
+dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical) | %resource.descendants().as(uri) | %resource.descendants().as(url))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}org-1:The organization SHALL at least have a name or an identifier, and possibly more than one {(identifier.count() + name.count()) &gt; 0}inv-dh-org-01:If present, the organization of which this organization forms a part shall at least have a reference, an identifier or a display {partOf.exists() implies (partOf.reference.exists() or partOf.identifier.exists() or partOf.display.exists())}</t>
   </si>
   <si>
     <t>(also see master files messages)</t>
@@ -389,8 +389,8 @@
     <t>National identifier Health Provider Identifier for Organisations (HPI-O).</t>
   </si>
   <si>
-    <t>inv-hpio-value-0:HPI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-hpio-value-1:HPI-O prefix is 800362 {value.startsWith('800362')}inv-hpio-value-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-hpio-0:HPI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
+inv-hpio-1:HPI-O prefix is 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Organization.identifier.id</t>
@@ -479,7 +479,7 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;system value="http://hl7.org.au/fhir/v2/0203"/&gt;
+    &lt;system value="http://terminology.hl7.org.au/CodeSystem/v2-0203"/&gt;
     &lt;code value="NOI"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
@@ -680,7 +680,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ABN (Australian Business Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-asic-abn-length:ABN shall be exactly 11 digits {value.length()=11}
+    <t xml:space="preserve">inv-abn-0:ABN shall be exactly 11 digits {value.length()=11}
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ACN (Australian Company Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-asic-acn-length:ACN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-acn-0:ACN shall be exactly 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -754,7 +754,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ARBN (Australian Registered Body Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-asic-arbn-length:ARBN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-arbn-0:ARBN shall be exactly 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -782,8 +782,8 @@
     <t>My Health Record Assigned Identity for Organisations (PAI-O).</t>
   </si>
   <si>
-    <t>inv-paio-value-0:PAI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-paio-value-1:PAI-O prefix is 800364 {value.startsWith('800364')}inv-paio-value-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-paio-0:PAI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
+inv-paio-1:PAI-O prefix is 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Identifier type for PAI-O</t>

</xml_diff>

<commit_message>
Published output of ES IG following updating to Guidance.  CIFMM-2767
</commit_message>
<xml_diff>
--- a/output/EventSummary/organization-dh-base-1.xlsx
+++ b/output/EventSummary/organization-dh-base-1.xlsx
@@ -389,8 +389,8 @@
     <t>National identifier Health Provider Identifier for Organisations (HPI-O).</t>
   </si>
   <si>
-    <t>inv-hpio-0:HPI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-hpio-1:HPI-O prefix is 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-hpio-0:HPI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
+inv-hpio-1:HPI-O prefix shall be 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Organization.identifier.id</t>
@@ -680,7 +680,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ABN (Australian Business Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-abn-0:ABN shall be exactly 11 digits {value.length()=11}
+    <t xml:space="preserve">inv-abn-0:ABN shall be 11 digits {value.length()=11}
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ACN (Australian Company Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-acn-0:ACN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-acn-0:ACN shall be 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -754,7 +754,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ARBN (Australian Registered Body Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-arbn-0:ARBN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-arbn-0:ARBN shall be 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -782,8 +782,8 @@
     <t>My Health Record Assigned Identity for Organisations (PAI-O).</t>
   </si>
   <si>
-    <t>inv-paio-0:PAI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-paio-1:PAI-O prefix is 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-paio-0:PAI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
+inv-paio-1:PAI-O prefix shall be 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Identifier type for PAI-O</t>
@@ -816,8 +816,8 @@
     <t xml:space="preserve">Contracted Service Provider (CSP) number identifier for organisations </t>
   </si>
   <si>
-    <t>inv-csp-0:CSP number is exactly 16 characters {value.length() = 16}
-inv-csp-1:CSP number prefix is 800363 {value.startsWith('800363')}</t>
+    <t>inv-csp-0:CSP number shall be 16 characters {value.length() = 16}
+inv-csp-1:CSP number prefix shall be 800363 {value.startsWith('800363')}</t>
   </si>
   <si>
     <t>Identifier type for CSP number</t>

</xml_diff>

<commit_message>
Regenerated ES Ig after making bugfixes to Disclaimers page.
</commit_message>
<xml_diff>
--- a/output/EventSummary/organization-dh-base-1.xlsx
+++ b/output/EventSummary/organization-dh-base-1.xlsx
@@ -389,8 +389,8 @@
     <t>National identifier Health Provider Identifier for Organisations (HPI-O).</t>
   </si>
   <si>
-    <t>inv-hpio-0:HPI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
-inv-hpio-1:HPI-O prefix shall be 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-hpio-0:HPI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
+inv-hpio-1:HPI-O prefix is 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Organization.identifier.id</t>
@@ -680,7 +680,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ABN (Australian Business Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-abn-0:ABN shall be 11 digits {value.length()=11}
+    <t xml:space="preserve">inv-abn-0:ABN shall be exactly 11 digits {value.length()=11}
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ACN (Australian Company Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-acn-0:ACN shall be 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-acn-0:ACN shall be exactly 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -754,7 +754,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ARBN (Australian Registered Body Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-arbn-0:ARBN shall be 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-arbn-0:ARBN shall be exactly 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -782,8 +782,8 @@
     <t>My Health Record Assigned Identity for Organisations (PAI-O).</t>
   </si>
   <si>
-    <t>inv-paio-0:PAI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
-inv-paio-1:PAI-O prefix shall be 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-paio-0:PAI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
+inv-paio-1:PAI-O prefix is 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Identifier type for PAI-O</t>
@@ -816,8 +816,8 @@
     <t xml:space="preserve">Contracted Service Provider (CSP) number identifier for organisations </t>
   </si>
   <si>
-    <t>inv-csp-0:CSP number shall be 16 characters {value.length() = 16}
-inv-csp-1:CSP number prefix shall be 800363 {value.startsWith('800363')}</t>
+    <t>inv-csp-0:CSP number is exactly 16 characters {value.length() = 16}
+inv-csp-1:CSP number prefix is 800363 {value.startsWith('800363')}</t>
   </si>
   <si>
     <t>Identifier type for CSP number</t>

</xml_diff>

<commit_message>
Regenerated outputs for Event Summary r4 which consists practitioner-dh-base profile.
CIFMM-2584
</commit_message>
<xml_diff>
--- a/output/EventSummary/organization-dh-base-1.xlsx
+++ b/output/EventSummary/organization-dh-base-1.xlsx
@@ -389,8 +389,8 @@
     <t>National identifier Health Provider Identifier for Organisations (HPI-O).</t>
   </si>
   <si>
-    <t>inv-hpio-0:HPI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-hpio-1:HPI-O prefix is 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-hpio-0:HPI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
+inv-hpio-1:HPI-O prefix shall be 800362 {value.startsWith('800362')}inv-hpio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Organization.identifier.id</t>
@@ -680,7 +680,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ABN (Australian Business Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-abn-0:ABN shall be exactly 11 digits {value.length()=11}
+    <t xml:space="preserve">inv-abn-0:ABN shall be 11 digits {value.length()=11}
 </t>
   </si>
   <si>
@@ -726,7 +726,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ACN (Australian Company Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-acn-0:ACN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-acn-0:ACN shall be 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -754,7 +754,7 @@
     <t>Australian Securities and Investment Commission (ASIC) assigned identifier for business/entity. ARBN (Australian Registered Body Number).</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-arbn-0:ARBN shall be exactly 9 digits {value.length()=9}
+    <t xml:space="preserve">inv-arbn-0:ARBN shall be 9 digits {value.length()=9}
 </t>
   </si>
   <si>
@@ -782,8 +782,8 @@
     <t>My Health Record Assigned Identity for Organisations (PAI-O).</t>
   </si>
   <si>
-    <t>inv-paio-0:PAI-O shall be an exactly 16 digit number {value.matches('^([0-9]{16})$')}
-inv-paio-1:PAI-O prefix is 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm check {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
+    <t>inv-paio-0:PAI-O shall be 16 digits {value.matches('^([0-9]{16})$')}
+inv-paio-1:PAI-O prefix shall be 800364 {value.startsWith('800364')}inv-paio-2:The identifier shall pass the Luhn algorithm {(((select(value.substring(0,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(1,1).toInteger())+(select(value.substring(2,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(3,1).toInteger())+(select(value.substring(4,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(5,1).toInteger())+(select(value.substring(6,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(7,1).toInteger())+(select(value.substring(8,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(9,1).toInteger())+(select(value.substring(10,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(11,1).toInteger())+(select(value.substring(12,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(13,1).toInteger())+(select(value.substring(14,1).toInteger()).select(iif($this&lt;5, $this*2, (($this*2)-9))))+(value.substring(15,1).toInteger()))mod 10=0)}</t>
   </si>
   <si>
     <t>Identifier type for PAI-O</t>
@@ -816,8 +816,8 @@
     <t xml:space="preserve">Contracted Service Provider (CSP) number identifier for organisations </t>
   </si>
   <si>
-    <t>inv-csp-0:CSP number is exactly 16 characters {value.length() = 16}
-inv-csp-1:CSP number prefix is 800363 {value.startsWith('800363')}</t>
+    <t>inv-csp-0:CSP number shall be 16 characters {value.length() = 16}
+inv-csp-1:CSP number prefix shall be 800363 {value.startsWith('800363')}</t>
   </si>
   <si>
     <t>Identifier type for CSP number</t>

</xml_diff>

<commit_message>
Corrected canonical urls in examples - Event Summary IG
</commit_message>
<xml_diff>
--- a/output/EventSummary/organization-dh-base-1.xlsx
+++ b/output/EventSummary/organization-dh-base-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="382">
   <si>
     <t>Path</t>
   </si>
@@ -146,7 +146,7 @@
     <t>*</t>
   </si>
   <si>
-    <t>An organisation in an Australian healthcare context</t>
+    <t>An organisation or an organisational unit</t>
   </si>
   <si>
     <t>A formally or informally recognized grouping of people or organizations formed for the purpose of achieving some form of collective action.  Includes companies, institutions, corporations, departments, community groups, healthcare practice groups, payer/insurer, etc.</t>
@@ -893,6 +893,9 @@
     <t>This resource is generally assumed to be active if no value is provided for the active element</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>No equivalent in HL7 v2</t>
   </si>
   <si>
@@ -1055,7 +1058,7 @@
     <t>Organization.partOf</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/4.0/StructureDefinition/organization-dh-base-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/StructureDefinition/organization-dh-base-1)
 </t>
   </si>
   <si>
@@ -12329,7 +12332,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
         <v>273</v>
       </c>
@@ -12345,7 +12348,7 @@
         <v>49</v>
       </c>
       <c r="G99" t="s" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H99" t="s" s="2">
         <v>50</v>
@@ -12375,7 +12378,7 @@
         <v>279</v>
       </c>
       <c r="Q99" t="s" s="2">
-        <v>40</v>
+        <v>280</v>
       </c>
       <c r="R99" t="s" s="2">
         <v>40</v>
@@ -12432,21 +12435,21 @@
         <v>61</v>
       </c>
       <c r="AJ99" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK99" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AL99" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM99" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
@@ -12472,16 +12475,16 @@
         <v>143</v>
       </c>
       <c r="K100" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="M100" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="N100" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="O100" t="s" s="2">
         <v>40</v>
@@ -12506,13 +12509,13 @@
         <v>40</v>
       </c>
       <c r="W100" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="X100" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Y100" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="Z100" t="s" s="2">
         <v>40</v>
@@ -12530,7 +12533,7 @@
         <v>40</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>41</v>
@@ -12545,21 +12548,21 @@
         <v>61</v>
       </c>
       <c r="AJ100" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AK100" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AL100" t="s" s="2">
         <v>126</v>
       </c>
       <c r="AM100" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
@@ -12585,16 +12588,16 @@
         <v>51</v>
       </c>
       <c r="K101" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L101" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M101" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="N101" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="O101" t="s" s="2">
         <v>40</v>
@@ -12643,7 +12646,7 @@
         <v>40</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>41</v>
@@ -12658,13 +12661,13 @@
         <v>61</v>
       </c>
       <c r="AJ101" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AK101" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AL101" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="AM101" t="s" s="2">
         <v>40</v>
@@ -12672,7 +12675,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -12698,16 +12701,16 @@
         <v>51</v>
       </c>
       <c r="K102" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="L102" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M102" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="N102" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="O102" t="s" s="2">
         <v>40</v>
@@ -12756,7 +12759,7 @@
         <v>40</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>41</v>
@@ -12774,7 +12777,7 @@
         <v>40</v>
       </c>
       <c r="AK102" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AL102" t="s" s="2">
         <v>40</v>
@@ -12785,7 +12788,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12808,19 +12811,19 @@
         <v>40</v>
       </c>
       <c r="J103" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K103" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="L103" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="M103" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N103" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O103" t="s" s="2">
         <v>40</v>
@@ -12869,7 +12872,7 @@
         <v>40</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>41</v>
@@ -12878,19 +12881,19 @@
         <v>42</v>
       </c>
       <c r="AH103" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="AI103" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AJ103" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AK103" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AL103" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="AM103" t="s" s="2">
         <v>40</v>
@@ -12898,7 +12901,7 @@
     </row>
     <row r="104">
       <c r="A104" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -12921,19 +12924,19 @@
         <v>40</v>
       </c>
       <c r="J104" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K104" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L104" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M104" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N104" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O104" t="s" s="2">
         <v>40</v>
@@ -12982,7 +12985,7 @@
         <v>40</v>
       </c>
       <c r="AE104" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF104" t="s" s="2">
         <v>41</v>
@@ -12991,19 +12994,19 @@
         <v>42</v>
       </c>
       <c r="AH104" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AI104" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AJ104" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AK104" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AL104" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AM104" t="s" s="2">
         <v>40</v>
@@ -13011,7 +13014,7 @@
     </row>
     <row r="105">
       <c r="A105" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -13034,17 +13037,17 @@
         <v>50</v>
       </c>
       <c r="J105" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="K105" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="L105" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="M105" s="2"/>
       <c r="N105" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="O105" t="s" s="2">
         <v>40</v>
@@ -13093,7 +13096,7 @@
         <v>40</v>
       </c>
       <c r="AE105" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="AF105" t="s" s="2">
         <v>41</v>
@@ -13108,10 +13111,10 @@
         <v>61</v>
       </c>
       <c r="AJ105" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK105" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AL105" t="s" s="2">
         <v>126</v>
@@ -13122,7 +13125,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13145,19 +13148,19 @@
         <v>40</v>
       </c>
       <c r="J106" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="L106" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="M106" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="N106" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="O106" t="s" s="2">
         <v>40</v>
@@ -13206,7 +13209,7 @@
         <v>40</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>41</v>
@@ -13224,7 +13227,7 @@
         <v>40</v>
       </c>
       <c r="AK106" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AL106" t="s" s="2">
         <v>40</v>
@@ -13235,7 +13238,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13344,7 +13347,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13455,11 +13458,11 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D109" s="2"/>
       <c r="E109" t="s" s="2">
@@ -13481,10 +13484,10 @@
         <v>95</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L109" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="M109" t="s" s="2">
         <v>98</v>
@@ -13539,7 +13542,7 @@
         <v>40</v>
       </c>
       <c r="AE109" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AF109" t="s" s="2">
         <v>41</v>
@@ -13568,7 +13571,7 @@
     </row>
     <row r="110">
       <c r="A110" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -13594,14 +13597,14 @@
         <v>143</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L110" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M110" s="2"/>
       <c r="N110" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O110" t="s" s="2">
         <v>40</v>
@@ -13629,10 +13632,10 @@
         <v>196</v>
       </c>
       <c r="X110" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="Y110" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="Z110" t="s" s="2">
         <v>40</v>
@@ -13650,7 +13653,7 @@
         <v>40</v>
       </c>
       <c r="AE110" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AF110" t="s" s="2">
         <v>41</v>
@@ -13668,7 +13671,7 @@
         <v>40</v>
       </c>
       <c r="AK110" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AL110" t="s" s="2">
         <v>40</v>
@@ -13679,7 +13682,7 @@
     </row>
     <row r="111">
       <c r="A111" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -13702,17 +13705,17 @@
         <v>40</v>
       </c>
       <c r="J111" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="K111" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="L111" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M111" s="2"/>
       <c r="N111" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="O111" t="s" s="2">
         <v>40</v>
@@ -13761,7 +13764,7 @@
         <v>40</v>
       </c>
       <c r="AE111" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AF111" t="s" s="2">
         <v>41</v>
@@ -13776,10 +13779,10 @@
         <v>61</v>
       </c>
       <c r="AJ111" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AK111" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AL111" t="s" s="2">
         <v>40</v>
@@ -13790,7 +13793,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13813,17 +13816,17 @@
         <v>40</v>
       </c>
       <c r="J112" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M112" s="2"/>
       <c r="N112" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O112" t="s" s="2">
         <v>40</v>
@@ -13872,7 +13875,7 @@
         <v>40</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>41</v>
@@ -13887,10 +13890,10 @@
         <v>61</v>
       </c>
       <c r="AJ112" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AK112" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AL112" t="s" s="2">
         <v>40</v>
@@ -13901,7 +13904,7 @@
     </row>
     <row r="113">
       <c r="A113" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -13924,17 +13927,17 @@
         <v>40</v>
       </c>
       <c r="J113" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K113" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M113" s="2"/>
       <c r="N113" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="O113" t="s" s="2">
         <v>40</v>
@@ -13983,7 +13986,7 @@
         <v>40</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>41</v>
@@ -13998,10 +14001,10 @@
         <v>61</v>
       </c>
       <c r="AJ113" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>40</v>
@@ -14012,7 +14015,7 @@
     </row>
     <row r="114" hidden="true">
       <c r="A114" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" t="s" s="2">
@@ -14035,17 +14038,17 @@
         <v>40</v>
       </c>
       <c r="J114" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="K114" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="L114" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M114" s="2"/>
       <c r="N114" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="O114" t="s" s="2">
         <v>40</v>
@@ -14094,7 +14097,7 @@
         <v>40</v>
       </c>
       <c r="AE114" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AF114" t="s" s="2">
         <v>41</v>

</xml_diff>